<commit_message>
add analysis for 2019.9 draft
</commit_message>
<xml_diff>
--- a/Outputs_figures/tab_TDA_alt_AL.xlsx
+++ b/Outputs_figures/tab_TDA_alt_AL.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>year</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t>MA.TDA_AL_multiTier_TDAamortAS_OYLM_TDA_LowRate1_lowG</t>
+  </si>
+  <si>
+    <t>MA.TDA_AL_multiTier_TDAamortAS_OYLM_TDA_LowRate2_base</t>
+  </si>
+  <si>
+    <t>MA.TDA_AL_multiTier_TDAamortAS_OYLM_TDA_LowRate2_lowG</t>
   </si>
   <si>
     <t>1</t>
@@ -83,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -109,10 +115,16 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>2016.0</v>
@@ -132,10 +144,16 @@
       <c r="G2" t="n">
         <v>0.2722982533414307</v>
       </c>
+      <c r="H2" t="n">
+        <v>0.2722982533414307</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.2722982533414307</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>2030.0</v>
@@ -155,10 +173,16 @@
       <c r="G3" t="n">
         <v>0.30715617440094867</v>
       </c>
+      <c r="H3" t="n">
+        <v>0.2507626990404917</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.21304163431459305</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>2048.0</v>
@@ -177,6 +201,12 @@
       </c>
       <c r="G4" t="n">
         <v>0.35327388262967274</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.2200181755456755</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1363696517206612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>